<commit_message>
dos correlation attack length tpr ratio
</commit_message>
<xml_diff>
--- a/visuals_dos_attack_length_stats.xlsx
+++ b/visuals_dos_attack_length_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\ids_svm_slidingwindow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4647DD41-680F-49EC-AD9F-A45081300ECE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398BD657-1008-4C3A-BD47-912F0C563B24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="330" windowWidth="24135" windowHeight="15090" xr2:uid="{160096AD-B1F0-47D3-B072-52F0427C5E47}"/>
+    <workbookView xWindow="3060" yWindow="750" windowWidth="24135" windowHeight="15090" xr2:uid="{160096AD-B1F0-47D3-B072-52F0427C5E47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Attack Length</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Pearson Correlation for attack length and Predicted Positive ratio</t>
+  </si>
+  <si>
+    <t>This measure says the longer the attack is, the better it does proportionally compared to baseline predicted positive ratio</t>
+  </si>
+  <si>
+    <t>This measure says the longer the attack is, the better internal TPR (PATPR) it will have</t>
   </si>
 </sst>
 </file>
@@ -521,6 +527,14 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Attack Length</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
                 <a:r>
                   <a:rPr lang="en-US"/>
                   <a:t>Second Threshold</a:t>
@@ -1090,6 +1104,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Attack Length (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1153,6 +1222,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>True</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Positve Rate (Per Attack)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1191,6 +1320,465 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="580288216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Predicted Positive Ratio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>502</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>901</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.663469804671383</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.21375710876570561</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3523182891343344</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.54613563952082966</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6005736455945812</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.811004263928192</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.1259843527920417</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.1341152669116612</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.8684840646887846</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.63952520583377082</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D7D6-40AA-8E3F-0EAE51E3E595}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="633871560"/>
+        <c:axId val="633869920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="633871560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="633869920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="633869920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="633871560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1306,6 +1894,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1810,6 +2438,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2394,6 +3538,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE39AB93-1BA8-4924-9FF9-636FDF741264}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2701,8 +3881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30B2A15-5A1C-4ED9-8828-3D4969ECA46A}">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,6 +3949,14 @@
       <c r="O2">
         <v>94</v>
       </c>
+      <c r="P2">
+        <f>(0/0.035212864)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>PEARSON(O2:O27,P2:P27)</f>
+        <v>0.39920375114808399</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2787,8 +3975,18 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
       <c r="O3">
         <v>206</v>
+      </c>
+      <c r="P3">
+        <f>(0/0.035212864)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -2811,6 +4009,10 @@
       <c r="O4">
         <v>100</v>
       </c>
+      <c r="P4">
+        <f>(0/0.035212864)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -2832,6 +4034,10 @@
       <c r="O5">
         <v>3</v>
       </c>
+      <c r="P5">
+        <f>(0/0.035212864)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2853,6 +4059,10 @@
       <c r="O6">
         <v>5</v>
       </c>
+      <c r="P6">
+        <f>(0/0.035212864)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -2874,6 +4084,10 @@
       <c r="O7">
         <v>618</v>
       </c>
+      <c r="P7">
+        <f>(0.97411/0.035212864)</f>
+        <v>27.663469804671383</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2895,6 +4109,10 @@
       <c r="O8">
         <v>930</v>
       </c>
+      <c r="P8">
+        <f>(0.007527/0.035212864)</f>
+        <v>0.21375710876570561</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2916,6 +4134,10 @@
       <c r="O9">
         <v>42</v>
       </c>
+      <c r="P9">
+        <f>(0.047619/0.035212864)</f>
+        <v>1.3523182891343344</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2937,6 +4159,10 @@
       <c r="O10">
         <v>2</v>
       </c>
+      <c r="P10">
+        <f>(0/0.035212864)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2958,6 +4184,10 @@
       <c r="O11">
         <v>10</v>
       </c>
+      <c r="P11">
+        <f>(0/0.035212864)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E12">
@@ -2969,6 +4199,10 @@
       <c r="O12">
         <v>46</v>
       </c>
+      <c r="P12">
+        <f>(0/0.035212864)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E13">
@@ -2980,6 +4214,10 @@
       <c r="O13">
         <v>52</v>
       </c>
+      <c r="P13">
+        <f>(0.019231/0.035212864)</f>
+        <v>0.54613563952082966</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E14">
@@ -2991,6 +4229,10 @@
       <c r="O14">
         <v>1</v>
       </c>
+      <c r="P14">
+        <f>0/0.78097</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E15">
@@ -3002,6 +4244,10 @@
       <c r="O15">
         <v>47</v>
       </c>
+      <c r="P15">
+        <f>(0/0.078097)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E16">
@@ -3013,8 +4259,12 @@
       <c r="O16">
         <v>608</v>
       </c>
+      <c r="P16">
+        <f>(0.125/0.078097)</f>
+        <v>1.6005736455945812</v>
+      </c>
     </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E17">
         <v>93</v>
       </c>
@@ -3024,8 +4274,12 @@
       <c r="O17">
         <v>93</v>
       </c>
+      <c r="P17">
+        <f>(0/0.078097)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E18">
         <v>502</v>
       </c>
@@ -3035,8 +4289,12 @@
       <c r="O18">
         <v>502</v>
       </c>
+      <c r="P18">
+        <f>(0.141434/0.078097)</f>
+        <v>1.811004263928192</v>
+      </c>
     </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>780</v>
       </c>
@@ -3046,8 +4304,12 @@
       <c r="O19">
         <v>780</v>
       </c>
+      <c r="P19">
+        <f>(0.634615/0.078097)</f>
+        <v>8.1259843527920417</v>
+      </c>
     </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>11</v>
       </c>
@@ -3057,8 +4319,12 @@
       <c r="O20">
         <v>11</v>
       </c>
+      <c r="P20">
+        <f>(0/0.078097)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E21">
         <v>2</v>
       </c>
@@ -3068,8 +4334,12 @@
       <c r="O21">
         <v>2</v>
       </c>
+      <c r="P21">
+        <f>(0/0.078097)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E22">
         <v>670</v>
       </c>
@@ -3079,8 +4349,12 @@
       <c r="O22">
         <v>670</v>
       </c>
+      <c r="P22">
+        <f>(0.088571/0.078097)</f>
+        <v>1.1341152669116612</v>
+      </c>
     </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E23">
         <v>1</v>
       </c>
@@ -3090,8 +4364,12 @@
       <c r="O23">
         <v>1</v>
       </c>
+      <c r="P23">
+        <f>(0/0.078097)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E24">
         <v>412</v>
       </c>
@@ -3101,8 +4379,12 @@
       <c r="O24">
         <v>412</v>
       </c>
+      <c r="P24">
+        <f>(0.536408/0.078097)</f>
+        <v>6.8684840646887846</v>
+      </c>
     </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>102</v>
       </c>
@@ -3112,8 +4394,12 @@
       <c r="O25">
         <v>102</v>
       </c>
+      <c r="P25">
+        <f>(0/0.078097)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>901</v>
       </c>
@@ -3123,8 +4409,12 @@
       <c r="O26">
         <v>901</v>
       </c>
+      <c r="P26">
+        <f>(0.049945/0.078097)</f>
+        <v>0.63952520583377082</v>
+      </c>
     </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>42</v>
       </c>
@@ -3133,6 +4423,10 @@
       </c>
       <c r="O27">
         <v>42</v>
+      </c>
+      <c r="P27">
+        <f>(0/0.078097)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>